<commit_message>
Update location processing and China Jesuit  communities mapping
Fixed many issues with the location processing and processing of Jesuit communities in China in 1644 according to Dehergne.
</commit_message>
<xml_diff>
--- a/inferences/jesuita-entrada-Coimbra-cargos_tarefas.datas.xlsx
+++ b/inferences/jesuita-entrada-Coimbra-cargos_tarefas.datas.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cargos_tarefas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="cargos_tarefas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1261,22 +1261,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Gaspar Ferreira</t>
+          <t>Francisco Vieira</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Mestre dos Noviços</t>
+          <t>Procurador</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1607</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1607</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1286,22 +1286,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>Francisco Vieira</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Superior da missão do Tonquim</t>
+          <t>Provincial de Goa</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1631</t>
+          <t>1609</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1631</t>
+          <t>1615</t>
         </is>
       </c>
     </row>
@@ -1311,22 +1311,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>Francisco Vieira</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1642</t>
+          <t>1615</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1645</t>
+          <t>1615</t>
         </is>
       </c>
     </row>
@@ -1336,22 +1336,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Gonçalo da Fonseca</t>
+          <t>Gaspar Ferreira</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Mestre dos Noviços</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1645</t>
+          <t>1607</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1660</t>
+          <t>1607</t>
         </is>
       </c>
     </row>
@@ -1361,22 +1361,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Gonçalo Álvares</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Visitador das Índias e do Japão</t>
+          <t>Superior da missão do Tonquim</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>1567</t>
+          <t>1631</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1567</t>
+          <t>1631</t>
         </is>
       </c>
     </row>
@@ -1386,22 +1386,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>José Montanha</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Procurador</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1753</t>
+          <t>1642</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1753</t>
+          <t>1645</t>
         </is>
       </c>
     </row>
@@ -1411,22 +1411,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>José Montanha</t>
+          <t>Gonçalo da Fonseca</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1749</t>
+          <t>1645</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1752</t>
+          <t>1660</t>
         </is>
       </c>
     </row>
@@ -1436,22 +1436,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>João da Rocha</t>
+          <t>Gonçalo Álvares</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Superior da missão da China</t>
+          <t>Visitador das Índias e do Japão</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1622</t>
+          <t>1567</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1622</t>
+          <t>1567</t>
         </is>
       </c>
     </row>
@@ -1461,22 +1461,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Leonardo Teixeira</t>
+          <t>José Montanha</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Procurador</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1753</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1753</t>
         </is>
       </c>
     </row>
@@ -1486,22 +1486,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>José Montanha</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Analista das missões da China e do Japão</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1583</t>
+          <t>1749</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1596</t>
+          <t>1752</t>
         </is>
       </c>
     </row>
@@ -1511,22 +1511,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>João da Rocha</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Monitor de Alessandro Valignano</t>
+          <t>Superior da missão da China</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1579</t>
+          <t>1622</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1579</t>
+          <t>1622</t>
         </is>
       </c>
     </row>
@@ -1536,22 +1536,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>Leonardo Teixeira</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Superior da residência de Macau</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1588</t>
+          <t>1699</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1588</t>
+          <t>1699</t>
         </is>
       </c>
     </row>
@@ -1561,22 +1561,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Analista das missões da China e do Japão</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>1583</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1654</t>
+          <t>1596</t>
         </is>
       </c>
     </row>
@@ -1586,22 +1586,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Visitador das missões</t>
+          <t>Monitor de Alessandro Valignano</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1614</t>
+          <t>1579</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1615</t>
+          <t>1579</t>
         </is>
       </c>
     </row>
@@ -1611,22 +1611,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Manuel Gaspar</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Procurador da China e do Japão</t>
+          <t>Superior da residência de Macau</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1603</t>
+          <t>1588</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1603</t>
+          <t>1588</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Manuel Mendes</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1646,12 +1646,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1714</t>
+          <t>1623</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1722</t>
+          <t>1654</t>
         </is>
       </c>
     </row>
@@ -1661,22 +1661,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Procurador da Província do Japão em Macau</t>
+          <t>Visitador das missões</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1614</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1615</t>
         </is>
       </c>
     </row>
@@ -1686,22 +1686,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Manuel Gaspar</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Reitor do colégio de Macau</t>
+          <t>Procurador da China e do Japão</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1603</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1603</t>
         </is>
       </c>
     </row>
@@ -1711,22 +1711,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Manuel Mendes</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1714</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1705</t>
+          <t>1722</t>
         </is>
       </c>
     </row>
@@ -1736,22 +1736,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Manuel de Sá</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Socius de Francesco Maria Spinola</t>
+          <t>Procurador da Província do Japão em Macau</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>1705</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>1705</t>
         </is>
       </c>
     </row>
@@ -1761,22 +1761,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Mateus de Couros</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Provincial do Japão e da China</t>
+          <t>Reitor do colégio de Macau</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1617</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1632</t>
+          <t>1704</t>
         </is>
       </c>
     </row>
@@ -1786,22 +1786,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1658</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1661</t>
+          <t>1705</t>
         </is>
       </c>
     </row>
@@ -1811,22 +1811,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Manuel de Sá</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Reitor do Colégio de Macau</t>
+          <t>Socius de Francesco Maria Spinola</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1694</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1694</t>
         </is>
       </c>
     </row>
@@ -1836,22 +1836,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Mateus de Couros</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Provincial do Japão e da China</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>1663</t>
+          <t>1617</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1666</t>
+          <t>1632</t>
         </is>
       </c>
     </row>
@@ -1866,17 +1866,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Vice-reitor do Colégio de Macau</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1651</t>
+          <t>1658</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1651</t>
+          <t>1661</t>
         </is>
       </c>
     </row>
@@ -1886,22 +1886,22 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Reitor do Colégio de Macau</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1694</t>
+          <t>1666</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1722</t>
+          <t>1666</t>
         </is>
       </c>
     </row>
@@ -1911,22 +1911,22 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1702</t>
+          <t>1663</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1718</t>
+          <t>1666</t>
         </is>
       </c>
     </row>
@@ -1936,22 +1936,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Vice-reitor do Colégio de Macau</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1719</t>
+          <t>1651</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1720</t>
+          <t>1651</t>
         </is>
       </c>
     </row>
@@ -1966,17 +1966,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Visitador da província de Goa</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>1704</t>
+          <t>1694</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1709</t>
+          <t>1722</t>
         </is>
       </c>
     </row>
@@ -1986,22 +1986,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Nicolau Pimenta</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Visitador das Índias Orientais</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1595</t>
+          <t>1702</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1613</t>
+          <t>1718</t>
         </is>
       </c>
     </row>
@@ -2011,22 +2011,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Pedro Martins</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Provincial das Índias Orientais</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1719</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1720</t>
         </is>
       </c>
     </row>
@@ -2036,22 +2036,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Pedro Martins</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Reitor de Goa</t>
+          <t>Visitador da província de Goa</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1704</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1586</t>
+          <t>1709</t>
         </is>
       </c>
     </row>
@@ -2061,22 +2061,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sebastião Vieira</t>
+          <t>Nicolau Pimenta</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Mestre dos Noviços</t>
+          <t>Visitador das Índias Orientais</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1604</t>
+          <t>1595</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1604</t>
+          <t>1613</t>
         </is>
       </c>
     </row>
@@ -2086,22 +2086,22 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Sebastião Vieira</t>
+          <t>Pedro Martins</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Procurador da província</t>
+          <t>Provincial das Índias Orientais</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>1586</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1623</t>
+          <t>1586</t>
         </is>
       </c>
     </row>
@@ -2111,22 +2111,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sebastião Vieira</t>
+          <t>Pedro Martins</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Secretário da Congregação Provincial do Japão</t>
+          <t>Reitor de Goa</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1619</t>
+          <t>1586</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1619</t>
+          <t>1586</t>
         </is>
       </c>
     </row>
@@ -2141,17 +2141,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Vice-provincial do Japão</t>
+          <t>Mestre dos Noviços</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1633</t>
+          <t>1604</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1634</t>
+          <t>1604</t>
         </is>
       </c>
     </row>
@@ -2161,22 +2161,22 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Sebastião da Maia</t>
+          <t>Sebastião Vieira</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Provincial do Japão</t>
+          <t>Procurador da província</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>1646</t>
+          <t>1623</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1649</t>
+          <t>1623</t>
         </is>
       </c>
     </row>
@@ -2186,22 +2186,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Sebastião da Maia</t>
+          <t>Sebastião Vieira</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Secretário da Congregação Provincial do Japão</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1650</t>
+          <t>1619</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1658</t>
+          <t>1619</t>
         </is>
       </c>
     </row>
@@ -2211,22 +2211,22 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Sebastião Vieira</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Procurador da Vice-província da China</t>
+          <t>Vice-provincial do Japão</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1633</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1658</t>
+          <t>1634</t>
         </is>
       </c>
     </row>
@@ -2236,22 +2236,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Sebastião da Maia</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Superior das residências de Kienning fou etc</t>
+          <t>Provincial do Japão</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1646</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1648</t>
+          <t>1649</t>
         </is>
       </c>
     </row>
@@ -2261,22 +2261,22 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Sebastião da Maia</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1657</t>
+          <t>1650</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1659</t>
+          <t>1658</t>
         </is>
       </c>
     </row>
@@ -2291,17 +2291,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Visitador do Japão e da China</t>
+          <t>Procurador da Vice-província da China</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1659</t>
+          <t>1648</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1660</t>
+          <t>1658</t>
         </is>
       </c>
     </row>
@@ -2311,22 +2311,22 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Provincial da Etiópia</t>
+          <t>Superior das residências de Kienning fou etc</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1555</t>
+          <t>1648</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1555</t>
+          <t>1648</t>
         </is>
       </c>
     </row>
@@ -2336,22 +2336,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Provincial das Índias Orientais</t>
+          <t>Vice-provincial da China</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1559</t>
+          <t>1657</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1572</t>
+          <t>1659</t>
         </is>
       </c>
     </row>
@@ -2361,22 +2361,22 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Superior da China</t>
+          <t>Visitador do Japão e da China</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1559</t>
+          <t>1659</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1572</t>
+          <t>1660</t>
         </is>
       </c>
     </row>
@@ -2391,17 +2391,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Vice-provincial das Índias Orientais</t>
+          <t>Provincial da Etiópia</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1556</t>
+          <t>1555</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1556</t>
+          <t>1555</t>
         </is>
       </c>
     </row>
@@ -2411,22 +2411,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Tomé (Sancho) Pereira</t>
+          <t>Tibúrcio de Quadros</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Vice-provincial da China</t>
+          <t>Provincial das Índias Orientais</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1692</t>
+          <t>1559</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1695</t>
+          <t>1572</t>
         </is>
       </c>
     </row>
@@ -2436,20 +2436,95 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
+          <t>Tibúrcio de Quadros</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Superior da China</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>1559</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>1572</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Tibúrcio de Quadros</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Vice-provincial das Índias Orientais</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>1556</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>1556</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>Tomé (Sancho) Pereira</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Vice-provincial da China</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>1692</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>1695</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Tomé (Sancho) Pereira</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
         <is>
           <t>Vice-visitador do Japão e da China</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>1691</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E84" t="inlineStr">
         <is>
           <t>1695</t>
         </is>

</xml_diff>